<commit_message>
Added a README sheet to the REMBI-template and the filled REMBI-template file.
</commit_message>
<xml_diff>
--- a/Topics/REMBI-Mapping/REMBI-template_CAi_VF.xlsx
+++ b/Topics/REMBI-Mapping/REMBI-template_CAi_VF.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vanes\NFDI4BIOIMAGE\REMBI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrea/repos/CEPLAS/NFDI4Bioimage/Cologne-Hackathon-2023/Topics/REMBI-Mapping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E010CA62-544D-428D-9181-CB47E7FCAC86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44731CC-79E6-234B-86C6-F2918ECCE2E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="3430" windowWidth="19420" windowHeight="10300" xr2:uid="{14919E20-F334-460A-AB37-8DA7FAC6926F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{14919E20-F334-460A-AB37-8DA7FAC6926F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Annotation template" sheetId="2" r:id="rId1"/>
-    <sheet name="K-v-pair layout" sheetId="3" r:id="rId2"/>
+    <sheet name="README" sheetId="4" r:id="rId1"/>
+    <sheet name="Annotation template" sheetId="2" r:id="rId2"/>
+    <sheet name="K-v-pair layout" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="48">
   <si>
     <r>
       <t xml:space="preserve">Annotation on the </t>
@@ -216,13 +217,152 @@
   </si>
   <si>
     <t>copyright</t>
+  </si>
+  <si>
+    <r>
+      <t>REMBI</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF171717"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF171717"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>RE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF171717"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>commended </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF171717"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF171717"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>etadata for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF171717"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>B</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF171717"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>iological </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF171717"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF171717"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>mages 
+The REMBI publication can be read here: https://rdcu.be/dsDc6.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>At the "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>NFDI4Bioimage - TA3-Hackathon - UoC-2023</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">", we used this REMBI-template which is used at CAi at HHU Duesseldorf.                                                           </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>CAi REMBI-template</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> is adapted from the REMBI table in the supplementary information of the REMBI publication: https://doi.org/10.1038/s41592-021-01166-8.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -246,8 +386,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF171717"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF171717"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -290,6 +456,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -304,7 +476,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -313,10 +485,22 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -332,7 +516,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -627,60 +811,109 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D18711-342F-BB47-9057-74937EA902A3}">
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="90.1640625" style="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="9"/>
+    </row>
+    <row r="3" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="9"/>
+    </row>
+    <row r="4" spans="1:1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="9"/>
+    </row>
+    <row r="6" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="79" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="10"/>
+    </row>
+    <row r="9" spans="1:1" ht="76" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="A6:A7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13B2F105-D05F-45B4-BF44-A816934754C1}">
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="42" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
@@ -688,25 +921,25 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>20</v>
       </c>
@@ -714,55 +947,55 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>22</v>
       </c>
@@ -770,49 +1003,49 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
       <c r="B23" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="B24" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
       <c r="B25" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
       <c r="B26" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
       <c r="B27" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
       <c r="B29" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>23</v>
       </c>
@@ -820,33 +1053,33 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="5"/>
       <c r="B31" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
         <v>38</v>
       </c>
@@ -863,7 +1096,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61805115-92CE-47FB-B1DA-F4E52C31E31A}">
   <dimension ref="A2:A34"/>
   <sheetViews>
@@ -871,169 +1104,172 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="41" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>19</v>
       </c>

</xml_diff>